<commit_message>
Updated till 13th Jan
</commit_message>
<xml_diff>
--- a/Data Science_Curriculum_Plan.xlsx
+++ b/Data Science_Curriculum_Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training'\DS\EKeeda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training'\eKeeda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B47964-B6AD-456B-98B4-D835553E3640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD61D5C-485E-474D-AF73-59AC0334E947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1018,7 +1021,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1058,6 +1061,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1232,8 +1241,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="45">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1291,50 +1300,22 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1351,11 +1332,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1619,7 +1631,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
@@ -1628,37 +1640,37 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="22">
         <v>6</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3">
         <v>1.2</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3">
         <v>1.3</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3">
@@ -1667,59 +1679,59 @@
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="22">
         <v>5</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3">
         <v>2.2000000000000002</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3">
         <v>2.4</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3">
         <v>2.5</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="3">
@@ -1728,68 +1740,68 @@
       <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="22">
         <v>6</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3">
         <v>3.2</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3">
         <v>3.3</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="3">
         <v>3.4</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="3">
         <v>3.5</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="3">
         <v>3.6</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="3">
@@ -1798,46 +1810,46 @@
       <c r="C17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="22">
         <v>4</v>
       </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="3">
         <v>4.2</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="3">
         <v>4.3</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="3">
@@ -1846,70 +1858,70 @@
       <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="22">
         <v>6</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="3">
         <v>5.2</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
     </row>
     <row r="23" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="3">
         <v>5.3</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="3">
         <v>5.4</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="3">
         <v>5.5</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="3">
         <v>5.6</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
     </row>
     <row r="27" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="3">
@@ -1918,37 +1930,37 @@
       <c r="C27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="26">
-        <v>3</v>
-      </c>
-      <c r="E27" s="23" t="s">
+      <c r="D27" s="22">
+        <v>3</v>
+      </c>
+      <c r="E27" s="25" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="3">
         <v>6.2</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
     </row>
     <row r="29" spans="1:5" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="3">
         <v>6.3</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="22" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="3">
@@ -1960,10 +1972,10 @@
       <c r="D30" s="3">
         <v>3</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="3">
         <v>7.2</v>
       </c>
@@ -1973,10 +1985,10 @@
       <c r="D31" s="3">
         <v>3</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="23"/>
     </row>
     <row r="32" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="3">
         <v>7.3</v>
       </c>
@@ -1986,10 +1998,10 @@
       <c r="D32" s="3">
         <v>3</v>
       </c>
-      <c r="E32" s="25"/>
+      <c r="E32" s="24"/>
     </row>
     <row r="33" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="3">
@@ -1998,70 +2010,70 @@
       <c r="C33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="22">
         <v>6</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="3">
         <v>8.1999999999999993</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="3">
         <v>8.4</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
     </row>
     <row r="37" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="3">
         <v>8.5</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
     </row>
     <row r="38" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="3">
         <v>8.6</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B39" s="3">
@@ -2070,68 +2082,68 @@
       <c r="C39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="26">
+      <c r="D39" s="22">
         <v>6</v>
       </c>
-      <c r="E39" s="24"/>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="3">
         <v>9.1999999999999993</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="3">
         <v>9.3000000000000007</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="3">
         <v>9.4</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="3">
         <v>9.5</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="3">
         <v>9.6</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="23"/>
     </row>
     <row r="45" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="22" t="s">
         <v>60</v>
       </c>
       <c r="B45" s="3">
@@ -2140,68 +2152,68 @@
       <c r="C45" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="22">
         <v>6</v>
       </c>
-      <c r="E45" s="24"/>
+      <c r="E45" s="23"/>
     </row>
     <row r="46" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="3">
         <v>10.199999999999999</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="3">
         <v>10.3</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
     </row>
     <row r="48" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="3">
         <v>10.4</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
     </row>
     <row r="49" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
+      <c r="A49" s="23"/>
       <c r="B49" s="3">
         <v>10.5</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="24"/>
       <c r="B50" s="3">
         <v>10.6</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="25"/>
-      <c r="E50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="23"/>
     </row>
     <row r="51" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="22" t="s">
         <v>67</v>
       </c>
       <c r="B51" s="3">
@@ -2210,35 +2222,35 @@
       <c r="C51" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="26">
+      <c r="D51" s="22">
         <v>6</v>
       </c>
-      <c r="E51" s="24"/>
+      <c r="E51" s="23"/>
     </row>
     <row r="52" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
+      <c r="A52" s="23"/>
       <c r="B52" s="3">
         <v>11.2</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
     </row>
     <row r="53" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="3">
         <v>11.3</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
     </row>
     <row r="54" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="22" t="s">
         <v>71</v>
       </c>
       <c r="B54" s="3">
@@ -2247,81 +2259,81 @@
       <c r="C54" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="26">
+      <c r="D54" s="22">
         <v>6</v>
       </c>
-      <c r="E54" s="26" t="s">
+      <c r="E54" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
+      <c r="A55" s="23"/>
       <c r="B55" s="3">
         <v>12.2</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
     </row>
     <row r="56" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="24"/>
+      <c r="A56" s="23"/>
       <c r="B56" s="3">
         <v>12.3</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="24"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="3">
         <v>12.4</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="24"/>
+      <c r="A58" s="23"/>
       <c r="B58" s="3">
         <v>12.5</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
     </row>
     <row r="59" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="24"/>
+      <c r="A59" s="23"/>
       <c r="B59" s="3">
         <v>12.6</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
     </row>
     <row r="60" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="3">
         <v>12.7</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
     </row>
     <row r="61" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B61" s="3">
@@ -2330,92 +2342,92 @@
       <c r="C61" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="26">
+      <c r="D61" s="22">
         <v>6</v>
       </c>
-      <c r="E61" s="26" t="s">
+      <c r="E61" s="22" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="3">
         <v>13.2</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
     </row>
     <row r="63" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="24"/>
+      <c r="A63" s="23"/>
       <c r="B63" s="3">
         <v>13.3</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
     </row>
     <row r="64" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="24"/>
+      <c r="A64" s="23"/>
       <c r="B64" s="3">
         <v>13.4</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
     </row>
     <row r="65" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="24"/>
+      <c r="A65" s="23"/>
       <c r="B65" s="3">
         <v>13.5</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
     </row>
     <row r="66" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="24"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="3">
         <v>13.6</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
     </row>
     <row r="67" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="24"/>
+      <c r="A67" s="23"/>
       <c r="B67" s="3">
         <v>13.7</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
     </row>
     <row r="68" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="3">
         <v>13.8</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
     </row>
     <row r="69" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="26" t="s">
+      <c r="A69" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B69" s="3">
@@ -2427,12 +2439,12 @@
       <c r="D69" s="3">
         <v>3</v>
       </c>
-      <c r="E69" s="23" t="s">
+      <c r="E69" s="25" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="3">
         <v>14.2</v>
       </c>
@@ -2442,10 +2454,10 @@
       <c r="D70" s="3">
         <v>3</v>
       </c>
-      <c r="E70" s="24"/>
+      <c r="E70" s="23"/>
     </row>
     <row r="71" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="24"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="3">
         <v>14.3</v>
       </c>
@@ -2455,10 +2467,10 @@
       <c r="D71" s="3">
         <v>2</v>
       </c>
-      <c r="E71" s="24"/>
+      <c r="E71" s="23"/>
     </row>
     <row r="72" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="24"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="3">
         <v>14.4</v>
       </c>
@@ -2468,10 +2480,10 @@
       <c r="D72" s="3">
         <v>2</v>
       </c>
-      <c r="E72" s="24"/>
+      <c r="E72" s="23"/>
     </row>
     <row r="73" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="24"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="3">
         <v>14.5</v>
       </c>
@@ -2481,10 +2493,10 @@
       <c r="D73" s="3">
         <v>2</v>
       </c>
-      <c r="E73" s="24"/>
+      <c r="E73" s="23"/>
     </row>
     <row r="74" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="3">
         <v>14.6</v>
       </c>
@@ -2494,7 +2506,7 @@
       <c r="D74" s="3">
         <v>3</v>
       </c>
-      <c r="E74" s="24"/>
+      <c r="E74" s="23"/>
     </row>
     <row r="75" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
@@ -2509,10 +2521,10 @@
       <c r="D75" s="3">
         <v>4</v>
       </c>
-      <c r="E75" s="24"/>
+      <c r="E75" s="23"/>
     </row>
     <row r="76" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="26" t="s">
+      <c r="A76" s="22" t="s">
         <v>100</v>
       </c>
       <c r="B76" s="3">
@@ -2524,10 +2536,10 @@
       <c r="D76" s="3">
         <v>3</v>
       </c>
-      <c r="E76" s="24"/>
+      <c r="E76" s="23"/>
     </row>
     <row r="77" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="24"/>
+      <c r="A77" s="23"/>
       <c r="B77" s="3">
         <v>15.2</v>
       </c>
@@ -2537,10 +2549,10 @@
       <c r="D77" s="3">
         <v>3</v>
       </c>
-      <c r="E77" s="24"/>
+      <c r="E77" s="23"/>
     </row>
     <row r="78" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="24"/>
+      <c r="A78" s="23"/>
       <c r="B78" s="3">
         <v>15.3</v>
       </c>
@@ -2550,10 +2562,10 @@
       <c r="D78" s="3">
         <v>3</v>
       </c>
-      <c r="E78" s="24"/>
+      <c r="E78" s="23"/>
     </row>
     <row r="79" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="24"/>
+      <c r="A79" s="23"/>
       <c r="B79" s="3">
         <v>15.4</v>
       </c>
@@ -2563,10 +2575,10 @@
       <c r="D79" s="3">
         <v>3</v>
       </c>
-      <c r="E79" s="24"/>
+      <c r="E79" s="23"/>
     </row>
     <row r="80" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="24"/>
+      <c r="A80" s="23"/>
       <c r="B80" s="3">
         <v>15.5</v>
       </c>
@@ -2576,10 +2588,10 @@
       <c r="D80" s="3">
         <v>3</v>
       </c>
-      <c r="E80" s="24"/>
+      <c r="E80" s="23"/>
     </row>
     <row r="81" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="25"/>
+      <c r="A81" s="24"/>
       <c r="B81" s="3">
         <v>15.6</v>
       </c>
@@ -2589,7 +2601,7 @@
       <c r="D81" s="3">
         <v>3</v>
       </c>
-      <c r="E81" s="24"/>
+      <c r="E81" s="23"/>
     </row>
     <row r="82" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
@@ -2604,10 +2616,10 @@
       <c r="D82" s="3">
         <v>4</v>
       </c>
-      <c r="E82" s="25"/>
+      <c r="E82" s="24"/>
     </row>
     <row r="83" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A83" s="26" t="s">
+      <c r="A83" s="22" t="s">
         <v>108</v>
       </c>
       <c r="B83" s="3">
@@ -2616,48 +2628,48 @@
       <c r="C83" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="26">
+      <c r="D83" s="22">
         <v>6</v>
       </c>
-      <c r="E83" s="23" t="s">
+      <c r="E83" s="25" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="24"/>
+      <c r="A84" s="23"/>
       <c r="B84" s="3">
         <v>16.2</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="24"/>
+      <c r="A85" s="23"/>
       <c r="B85" s="3">
         <v>16.3</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="25"/>
+      <c r="A86" s="24"/>
       <c r="B86" s="3">
         <v>16.399999999999999</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D86" s="25"/>
-      <c r="E86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="23"/>
     </row>
     <row r="87" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A87" s="26" t="s">
+      <c r="A87" s="22" t="s">
         <v>114</v>
       </c>
       <c r="B87" s="3">
@@ -2669,10 +2681,10 @@
       <c r="D87" s="3">
         <v>3</v>
       </c>
-      <c r="E87" s="24"/>
+      <c r="E87" s="23"/>
     </row>
     <row r="88" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="24"/>
+      <c r="A88" s="23"/>
       <c r="B88" s="3">
         <v>17.2</v>
       </c>
@@ -2682,10 +2694,10 @@
       <c r="D88" s="3">
         <v>3</v>
       </c>
-      <c r="E88" s="24"/>
+      <c r="E88" s="23"/>
     </row>
     <row r="89" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
+      <c r="A89" s="24"/>
       <c r="B89" s="3">
         <v>17.3</v>
       </c>
@@ -2695,7 +2707,7 @@
       <c r="D89" s="3">
         <v>3</v>
       </c>
-      <c r="E89" s="24"/>
+      <c r="E89" s="23"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
@@ -2710,10 +2722,10 @@
       <c r="D90" s="3">
         <v>4</v>
       </c>
-      <c r="E90" s="25"/>
+      <c r="E90" s="24"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="26" t="s">
+      <c r="A91" s="22" t="s">
         <v>119</v>
       </c>
       <c r="B91" s="3">
@@ -2722,81 +2734,81 @@
       <c r="C91" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D91" s="26">
+      <c r="D91" s="22">
         <v>6</v>
       </c>
-      <c r="E91" s="23" t="s">
+      <c r="E91" s="25" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="24"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="3">
         <v>18.2</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="24"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="3">
         <v>18.3</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="24"/>
+      <c r="A94" s="23"/>
       <c r="B94" s="3">
         <v>18.399999999999999</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D94" s="24"/>
-      <c r="E94" s="24"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
     </row>
     <row r="95" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="24"/>
+      <c r="A95" s="23"/>
       <c r="B95" s="3">
         <v>18.5</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D95" s="24"/>
-      <c r="E95" s="24"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="24"/>
+      <c r="A96" s="23"/>
       <c r="B96" s="3">
         <v>18.600000000000001</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
     </row>
     <row r="97" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
+      <c r="A97" s="24"/>
       <c r="B97" s="3">
         <v>18.7</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D97" s="25"/>
-      <c r="E97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="23"/>
     </row>
     <row r="98" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="26" t="s">
+      <c r="A98" s="22" t="s">
         <v>128</v>
       </c>
       <c r="B98" s="3">
@@ -2805,35 +2817,35 @@
       <c r="C98" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D98" s="26">
-        <v>3</v>
-      </c>
-      <c r="E98" s="24"/>
+      <c r="D98" s="22">
+        <v>3</v>
+      </c>
+      <c r="E98" s="23"/>
     </row>
     <row r="99" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="24"/>
+      <c r="A99" s="23"/>
       <c r="B99" s="3">
         <v>19.2</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D99" s="24"/>
-      <c r="E99" s="24"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
     </row>
     <row r="100" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="25"/>
+      <c r="A100" s="24"/>
       <c r="B100" s="3">
         <v>19.3</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
     </row>
     <row r="101" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="22" t="s">
         <v>132</v>
       </c>
       <c r="B101" s="3">
@@ -2842,37 +2854,37 @@
       <c r="C101" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D101" s="26">
-        <v>3</v>
-      </c>
-      <c r="E101" s="23" t="s">
+      <c r="D101" s="22">
+        <v>3</v>
+      </c>
+      <c r="E101" s="25" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="24"/>
+      <c r="A102" s="23"/>
       <c r="B102" s="3">
         <v>20.2</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D102" s="24"/>
-      <c r="E102" s="24"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="23"/>
     </row>
     <row r="103" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="25"/>
+      <c r="A103" s="24"/>
       <c r="B103" s="3">
         <v>20.3</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D103" s="25"/>
-      <c r="E103" s="24"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="23"/>
     </row>
     <row r="104" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="26" t="s">
+      <c r="A104" s="22" t="s">
         <v>137</v>
       </c>
       <c r="B104" s="3">
@@ -2881,57 +2893,57 @@
       <c r="C104" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D104" s="26">
+      <c r="D104" s="22">
         <v>6</v>
       </c>
-      <c r="E104" s="24"/>
+      <c r="E104" s="23"/>
     </row>
     <row r="105" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="24"/>
+      <c r="A105" s="23"/>
       <c r="B105" s="3">
         <v>21.2</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D105" s="24"/>
-      <c r="E105" s="24"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="23"/>
     </row>
     <row r="106" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="24"/>
+      <c r="A106" s="23"/>
       <c r="B106" s="3">
         <v>21.3</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D106" s="24"/>
-      <c r="E106" s="24"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
     </row>
     <row r="107" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="24"/>
+      <c r="A107" s="23"/>
       <c r="B107" s="3">
         <v>21.4</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D107" s="24"/>
-      <c r="E107" s="24"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="23"/>
     </row>
     <row r="108" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="25"/>
+      <c r="A108" s="24"/>
       <c r="B108" s="3">
         <v>21.5</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D108" s="25"/>
-      <c r="E108" s="25"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="24"/>
     </row>
     <row r="109" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="26" t="s">
+      <c r="A109" s="22" t="s">
         <v>143</v>
       </c>
       <c r="B109" s="3">
@@ -2940,59 +2952,59 @@
       <c r="C109" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D109" s="26">
+      <c r="D109" s="22">
         <v>6</v>
       </c>
-      <c r="E109" s="23" t="s">
+      <c r="E109" s="25" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="24"/>
+      <c r="A110" s="23"/>
       <c r="B110" s="3">
         <v>22.2</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D110" s="24"/>
-      <c r="E110" s="24"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
     </row>
     <row r="111" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="24"/>
+      <c r="A111" s="23"/>
       <c r="B111" s="3">
         <v>22.3</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="23"/>
     </row>
     <row r="112" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="24"/>
+      <c r="A112" s="23"/>
       <c r="B112" s="3">
         <v>22.4</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D112" s="24"/>
-      <c r="E112" s="24"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="23"/>
     </row>
     <row r="113" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="25"/>
+      <c r="A113" s="24"/>
       <c r="B113" s="3">
         <v>22.5</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D113" s="25"/>
-      <c r="E113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="23"/>
     </row>
     <row r="114" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="26" t="s">
+      <c r="A114" s="22" t="s">
         <v>150</v>
       </c>
       <c r="B114" s="3">
@@ -3001,43 +3013,43 @@
       <c r="C114" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D114" s="26">
+      <c r="D114" s="22">
         <v>6</v>
       </c>
-      <c r="E114" s="24"/>
+      <c r="E114" s="23"/>
     </row>
     <row r="115" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="24"/>
+      <c r="A115" s="23"/>
       <c r="B115" s="3">
         <v>23.2</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D115" s="24"/>
-      <c r="E115" s="24"/>
+      <c r="D115" s="23"/>
+      <c r="E115" s="23"/>
     </row>
     <row r="116" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="24"/>
+      <c r="A116" s="23"/>
       <c r="B116" s="3">
         <v>23.3</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
+      <c r="D116" s="23"/>
+      <c r="E116" s="23"/>
     </row>
     <row r="117" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="25"/>
+      <c r="A117" s="24"/>
       <c r="B117" s="3">
         <v>23.4</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D117" s="25"/>
-      <c r="E117" s="24"/>
+      <c r="D117" s="24"/>
+      <c r="E117" s="23"/>
     </row>
     <row r="118" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
@@ -3052,10 +3064,10 @@
       <c r="D118" s="3">
         <v>3</v>
       </c>
-      <c r="E118" s="25"/>
+      <c r="E118" s="24"/>
     </row>
     <row r="119" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="26" t="s">
+      <c r="A119" s="22" t="s">
         <v>156</v>
       </c>
       <c r="B119" s="3">
@@ -3064,70 +3076,70 @@
       <c r="C119" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D119" s="26">
+      <c r="D119" s="22">
         <v>6</v>
       </c>
-      <c r="E119" s="23" t="s">
+      <c r="E119" s="25" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="24"/>
+      <c r="A120" s="23"/>
       <c r="B120" s="3">
         <v>24.2</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D120" s="24"/>
-      <c r="E120" s="24"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="23"/>
     </row>
     <row r="121" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="24"/>
+      <c r="A121" s="23"/>
       <c r="B121" s="3">
         <v>24.3</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D121" s="24"/>
-      <c r="E121" s="24"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
     </row>
     <row r="122" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A122" s="24"/>
+      <c r="A122" s="23"/>
       <c r="B122" s="3">
         <v>24.4</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D122" s="24"/>
-      <c r="E122" s="24"/>
+      <c r="D122" s="23"/>
+      <c r="E122" s="23"/>
     </row>
     <row r="123" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="24"/>
+      <c r="A123" s="23"/>
       <c r="B123" s="3">
         <v>24.5</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D123" s="24"/>
-      <c r="E123" s="24"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="23"/>
     </row>
     <row r="124" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A124" s="25"/>
+      <c r="A124" s="24"/>
       <c r="B124" s="3">
         <v>24.6</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D124" s="25"/>
-      <c r="E124" s="24"/>
+      <c r="D124" s="24"/>
+      <c r="E124" s="23"/>
     </row>
     <row r="125" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="26" t="s">
+      <c r="A125" s="22" t="s">
         <v>164</v>
       </c>
       <c r="B125" s="3">
@@ -3136,35 +3148,35 @@
       <c r="C125" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D125" s="26">
+      <c r="D125" s="22">
         <v>6</v>
       </c>
-      <c r="E125" s="24"/>
+      <c r="E125" s="23"/>
     </row>
     <row r="126" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A126" s="24"/>
+      <c r="A126" s="23"/>
       <c r="B126" s="3">
         <v>25.2</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D126" s="24"/>
-      <c r="E126" s="24"/>
+      <c r="D126" s="23"/>
+      <c r="E126" s="23"/>
     </row>
     <row r="127" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="24"/>
+      <c r="A127" s="23"/>
       <c r="B127" s="3">
         <v>25.3</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D127" s="25"/>
-      <c r="E127" s="24"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="23"/>
     </row>
     <row r="128" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="25"/>
+      <c r="A128" s="24"/>
       <c r="B128" s="3">
         <v>25.4</v>
       </c>
@@ -3174,10 +3186,10 @@
       <c r="D128" s="3">
         <v>3</v>
       </c>
-      <c r="E128" s="25"/>
+      <c r="E128" s="24"/>
     </row>
     <row r="129" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="26" t="s">
+      <c r="A129" s="22" t="s">
         <v>169</v>
       </c>
       <c r="B129" s="3">
@@ -3186,37 +3198,37 @@
       <c r="C129" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D129" s="26">
+      <c r="D129" s="22">
         <v>6</v>
       </c>
-      <c r="E129" s="26" t="s">
+      <c r="E129" s="22" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="24"/>
+      <c r="A130" s="23"/>
       <c r="B130" s="3">
         <v>26.2</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D130" s="24"/>
-      <c r="E130" s="24"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="23"/>
     </row>
     <row r="131" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="25"/>
+      <c r="A131" s="24"/>
       <c r="B131" s="3">
         <v>26.3</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D131" s="25"/>
-      <c r="E131" s="25"/>
+      <c r="D131" s="24"/>
+      <c r="E131" s="24"/>
     </row>
     <row r="132" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="26" t="s">
+      <c r="A132" s="22" t="s">
         <v>174</v>
       </c>
       <c r="B132" s="3">
@@ -3228,12 +3240,12 @@
       <c r="D132" s="3">
         <v>5</v>
       </c>
-      <c r="E132" s="23" t="s">
+      <c r="E132" s="25" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A133" s="25"/>
+      <c r="A133" s="24"/>
       <c r="B133" s="3">
         <v>27.2</v>
       </c>
@@ -3243,58 +3255,10 @@
       <c r="D133" s="3">
         <v>10</v>
       </c>
-      <c r="E133" s="25"/>
+      <c r="E133" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E33:E53"/>
-    <mergeCell ref="D45:D50"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E6:E20"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="D119:D124"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="E119:E128"/>
-    <mergeCell ref="A125:A128"/>
-    <mergeCell ref="D125:D127"/>
-    <mergeCell ref="D129:D131"/>
-    <mergeCell ref="E129:E131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A119:A124"/>
-    <mergeCell ref="A129:A131"/>
-    <mergeCell ref="D91:D97"/>
-    <mergeCell ref="E91:E100"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="D98:D100"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="A114:A117"/>
-    <mergeCell ref="E101:E108"/>
-    <mergeCell ref="D109:D113"/>
-    <mergeCell ref="E109:E118"/>
-    <mergeCell ref="D114:D117"/>
-    <mergeCell ref="D101:D103"/>
-    <mergeCell ref="D104:D108"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="A61:A68"/>
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A91:A97"/>
-    <mergeCell ref="A76:A81"/>
     <mergeCell ref="E83:E90"/>
     <mergeCell ref="A87:A89"/>
     <mergeCell ref="D83:D86"/>
@@ -3311,6 +3275,54 @@
     <mergeCell ref="E61:E68"/>
     <mergeCell ref="E69:E82"/>
     <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A61:A68"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A91:A97"/>
+    <mergeCell ref="A76:A81"/>
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="E101:E108"/>
+    <mergeCell ref="D109:D113"/>
+    <mergeCell ref="E109:E118"/>
+    <mergeCell ref="D114:D117"/>
+    <mergeCell ref="D101:D103"/>
+    <mergeCell ref="D104:D108"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="D91:D97"/>
+    <mergeCell ref="E91:E100"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="D119:D124"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="E119:E128"/>
+    <mergeCell ref="A125:A128"/>
+    <mergeCell ref="D125:D127"/>
+    <mergeCell ref="D129:D131"/>
+    <mergeCell ref="E129:E131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A119:A124"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E20"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E33:E53"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="D51:D53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3321,7 +3333,7 @@
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="G45" sqref="G45:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.25"/>
@@ -3364,7 +3376,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="41">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
       <c r="B2" s="10">
@@ -3382,15 +3394,15 @@
       <c r="F2" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="8">
         <v>44765</v>
       </c>
@@ -3406,13 +3418,13 @@
       <c r="F3" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="22" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="21" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="8">
         <v>44766</v>
       </c>
@@ -3428,13 +3440,13 @@
       <c r="F4" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="22" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="21" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
+      <c r="A5" s="26">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3452,15 +3464,15 @@
       <c r="F5" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="6" t="s">
         <v>186</v>
       </c>
@@ -3476,13 +3488,13 @@
       <c r="F6" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="22" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="21" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="6" t="s">
         <v>187</v>
       </c>
@@ -3498,15 +3510,15 @@
       <c r="F7" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
+      <c r="A8" s="26">
         <v>3</v>
       </c>
       <c r="B8" s="9">
@@ -3524,13 +3536,13 @@
       <c r="F8" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="22" t="s">
+      <c r="G8" s="32"/>
+      <c r="H8" s="21" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="9">
         <v>44720</v>
       </c>
@@ -3546,13 +3558,13 @@
       <c r="F9" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="22" t="s">
+      <c r="G9" s="32"/>
+      <c r="H9" s="21" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="9">
         <v>44750</v>
       </c>
@@ -3568,15 +3580,15 @@
       <c r="F10" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="21" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="42">
+      <c r="A11" s="26">
         <v>4</v>
       </c>
       <c r="B11" s="9">
@@ -3594,13 +3606,13 @@
       <c r="F11" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="22" t="s">
+      <c r="G11" s="32"/>
+      <c r="H11" s="21" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="6" t="s">
         <v>188</v>
       </c>
@@ -3616,15 +3628,15 @@
       <c r="F12" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="39" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="6" t="s">
         <v>189</v>
       </c>
@@ -3640,13 +3652,13 @@
       <c r="F13" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="15" t="s">
+      <c r="G13" s="32"/>
+      <c r="H13" s="39" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A14" s="42">
+      <c r="A14" s="26">
         <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3664,15 +3676,15 @@
       <c r="F14" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="39" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="6" t="s">
         <v>191</v>
       </c>
@@ -3688,13 +3700,13 @@
       <c r="F15" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="15" t="s">
+      <c r="G15" s="36"/>
+      <c r="H15" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="6" t="s">
         <v>192</v>
       </c>
@@ -3710,15 +3722,15 @@
       <c r="F16" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="39" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="42">
+      <c r="A17" s="26">
         <v>6</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -3736,13 +3748,13 @@
       <c r="F17" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="15" t="s">
+      <c r="G17" s="32"/>
+      <c r="H17" s="39" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="6" t="s">
         <v>194</v>
       </c>
@@ -3758,13 +3770,13 @@
       <c r="F18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="32" t="s">
+      <c r="G18" s="32"/>
+      <c r="H18" s="40" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="6" t="s">
         <v>195</v>
       </c>
@@ -3780,11 +3792,11 @@
       <c r="F19" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="33"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="42">
+      <c r="A20" s="26">
         <v>7</v>
       </c>
       <c r="B20" s="9">
@@ -3802,15 +3814,15 @@
       <c r="F20" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="39" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="9">
         <v>44629</v>
       </c>
@@ -3826,13 +3838,13 @@
       <c r="F21" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="20" t="s">
+      <c r="G21" s="32"/>
+      <c r="H21" s="39" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="9">
         <v>44660</v>
       </c>
@@ -3848,15 +3860,15 @@
       <c r="F22" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="39" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A23" s="42">
+      <c r="A23" s="26">
         <v>8</v>
       </c>
       <c r="B23" s="9">
@@ -3874,13 +3886,13 @@
       <c r="F23" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="20" t="s">
+      <c r="G23" s="32"/>
+      <c r="H23" s="39" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="9">
         <v>44843</v>
       </c>
@@ -3896,15 +3908,15 @@
       <c r="F24" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="39" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="9">
         <v>44874</v>
       </c>
@@ -3920,13 +3932,13 @@
       <c r="F25" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="20" t="s">
+      <c r="G25" s="32"/>
+      <c r="H25" s="39" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A26" s="42">
+      <c r="A26" s="26">
         <v>9</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -3944,15 +3956,15 @@
       <c r="F26" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G26" s="30" t="s">
+      <c r="G26" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H26" s="39" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="6" t="s">
         <v>197</v>
       </c>
@@ -3968,13 +3980,13 @@
       <c r="F27" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="20" t="s">
+      <c r="G27" s="32"/>
+      <c r="H27" s="39" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="6" t="s">
         <v>198</v>
       </c>
@@ -3990,15 +4002,15 @@
       <c r="F28" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="39" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="42">
+      <c r="A29" s="26">
         <v>10</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -4016,13 +4028,13 @@
       <c r="F29" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="20" t="s">
+      <c r="G29" s="34"/>
+      <c r="H29" s="39" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="6" t="s">
         <v>200</v>
       </c>
@@ -4038,13 +4050,13 @@
       <c r="F30" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="20" t="s">
+      <c r="G30" s="34"/>
+      <c r="H30" s="39" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="6" t="s">
         <v>201</v>
       </c>
@@ -4060,13 +4072,13 @@
       <c r="F31" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="20" t="s">
+      <c r="G31" s="34"/>
+      <c r="H31" s="39" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="42">
+      <c r="A32" s="26">
         <v>11</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -4084,13 +4096,13 @@
       <c r="F32" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G32" s="28"/>
-      <c r="H32" s="20" t="s">
+      <c r="G32" s="34"/>
+      <c r="H32" s="39" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="9">
         <v>44571</v>
       </c>
@@ -4106,13 +4118,13 @@
       <c r="F33" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G33" s="28"/>
-      <c r="H33" s="20" t="s">
+      <c r="G33" s="34"/>
+      <c r="H33" s="39" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="9">
         <v>44602</v>
       </c>
@@ -4131,12 +4143,12 @@
       <c r="G34" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="42" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="42">
+      <c r="A35" s="26">
         <v>12</v>
       </c>
       <c r="B35" s="9">
@@ -4154,15 +4166,15 @@
       <c r="F35" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="39" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="9">
         <v>44783</v>
       </c>
@@ -4178,13 +4190,13 @@
       <c r="F36" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="20" t="s">
+      <c r="G36" s="32"/>
+      <c r="H36" s="39" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="9">
         <v>44814</v>
       </c>
@@ -4200,13 +4212,13 @@
       <c r="F37" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G37" s="30"/>
-      <c r="H37" s="20" t="s">
+      <c r="G37" s="32"/>
+      <c r="H37" s="39" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="42">
+      <c r="A38" s="26">
         <v>13</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -4224,13 +4236,13 @@
       <c r="F38" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G38" s="30"/>
-      <c r="H38" s="20" t="s">
+      <c r="G38" s="32"/>
+      <c r="H38" s="39" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="6" t="s">
         <v>204</v>
       </c>
@@ -4246,13 +4258,13 @@
       <c r="F39" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="H39" s="20" t="s">
+      <c r="G39" s="32"/>
+      <c r="H39" s="39" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="6" t="s">
         <v>205</v>
       </c>
@@ -4268,13 +4280,13 @@
       <c r="F40" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G40" s="30"/>
-      <c r="H40" s="20" t="s">
+      <c r="G40" s="32"/>
+      <c r="H40" s="39" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="42">
+      <c r="A41" s="26">
         <v>14</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -4292,15 +4304,15 @@
       <c r="F41" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G41" s="34" t="s">
+      <c r="G41" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H41" s="35" t="s">
+      <c r="H41" s="43" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="6" t="s">
         <v>207</v>
       </c>
@@ -4316,11 +4328,11 @@
       <c r="F42" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G42" s="34"/>
-      <c r="H42" s="36"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="44"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="6" t="s">
         <v>208</v>
       </c>
@@ -4336,15 +4348,15 @@
       <c r="F43" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G43" s="30" t="s">
+      <c r="G43" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="39" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="42">
+      <c r="A44" s="26">
         <v>15</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -4362,13 +4374,13 @@
       <c r="F44" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G44" s="30"/>
-      <c r="H44" s="20" t="s">
+      <c r="G44" s="32"/>
+      <c r="H44" s="39" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="6" t="s">
         <v>210</v>
       </c>
@@ -4384,15 +4396,15 @@
       <c r="F45" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G45" s="30" t="s">
+      <c r="G45" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="39" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="6" t="s">
         <v>211</v>
       </c>
@@ -4408,13 +4420,13 @@
       <c r="F46" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G46" s="30"/>
-      <c r="H46" s="20" t="s">
+      <c r="G46" s="32"/>
+      <c r="H46" s="39" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="42">
+      <c r="A47" s="26">
         <v>16</v>
       </c>
       <c r="B47" s="9">
@@ -4432,13 +4444,13 @@
       <c r="F47" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G47" s="30"/>
-      <c r="H47" s="20" t="s">
+      <c r="G47" s="32"/>
+      <c r="H47" s="39" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="9">
         <v>44692</v>
       </c>
@@ -4462,7 +4474,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="42"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="9">
         <v>44723</v>
       </c>
@@ -4478,15 +4490,15 @@
       <c r="F49" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G49" s="30" t="s">
+      <c r="G49" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="H49" s="20" t="s">
+      <c r="H49" s="39" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="42">
+      <c r="A50" s="26">
         <v>17</v>
       </c>
       <c r="B50" s="9">
@@ -4504,13 +4516,13 @@
       <c r="F50" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G50" s="30"/>
-      <c r="H50" s="20" t="s">
+      <c r="G50" s="32"/>
+      <c r="H50" s="39" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="9">
         <v>44906</v>
       </c>
@@ -4526,13 +4538,13 @@
       <c r="F51" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G51" s="30"/>
-      <c r="H51" s="20" t="s">
+      <c r="G51" s="32"/>
+      <c r="H51" s="39" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="42"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="6" t="s">
         <v>212</v>
       </c>
@@ -4548,13 +4560,13 @@
       <c r="F52" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G52" s="30"/>
-      <c r="H52" s="20" t="s">
+      <c r="G52" s="32"/>
+      <c r="H52" s="39" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="42">
+      <c r="A53" s="26">
         <v>18</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -4572,15 +4584,15 @@
       <c r="F53" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G53" s="30" t="s">
+      <c r="G53" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="H53" s="20" t="s">
+      <c r="H53" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="42"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="6" t="s">
         <v>214</v>
       </c>
@@ -4596,13 +4608,13 @@
       <c r="F54" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G54" s="30"/>
-      <c r="H54" s="20" t="s">
+      <c r="G54" s="32"/>
+      <c r="H54" s="15" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="42"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="6" t="s">
         <v>215</v>
       </c>
@@ -4618,13 +4630,13 @@
       <c r="F55" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G55" s="30"/>
-      <c r="H55" s="20" t="s">
+      <c r="G55" s="32"/>
+      <c r="H55" s="15" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="42">
+      <c r="A56" s="26">
         <v>19</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -4642,11 +4654,11 @@
       <c r="F56" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G56" s="30"/>
+      <c r="G56" s="32"/>
       <c r="H56" s="15"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="42"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="6" t="s">
         <v>217</v>
       </c>
@@ -4670,7 +4682,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="6" t="s">
         <v>218</v>
       </c>
@@ -4694,7 +4706,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="42">
+      <c r="A59" s="26">
         <v>20</v>
       </c>
       <c r="B59" s="9">
@@ -4712,7 +4724,7 @@
       <c r="F59" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G59" s="30" t="s">
+      <c r="G59" s="32" t="s">
         <v>67</v>
       </c>
       <c r="H59" s="15" t="s">
@@ -4720,7 +4732,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="42"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="9">
         <v>44632</v>
       </c>
@@ -4736,13 +4748,13 @@
       <c r="F60" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G60" s="30"/>
+      <c r="G60" s="32"/>
       <c r="H60" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="42"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="9">
         <v>44663</v>
       </c>
@@ -4758,7 +4770,7 @@
       <c r="F61" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G61" s="30" t="s">
+      <c r="G61" s="32" t="s">
         <v>119</v>
       </c>
       <c r="H61" s="15" t="s">
@@ -4766,7 +4778,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="42">
+      <c r="A62" s="26">
         <v>21</v>
       </c>
       <c r="B62" s="9">
@@ -4784,13 +4796,13 @@
       <c r="F62" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G62" s="30"/>
+      <c r="G62" s="32"/>
       <c r="H62" s="15" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="42"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="9">
         <v>44846</v>
       </c>
@@ -4814,7 +4826,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="42"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="9">
         <v>44877</v>
       </c>
@@ -4838,7 +4850,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="42">
+      <c r="A65" s="26">
         <v>22</v>
       </c>
       <c r="B65" s="6" t="s">
@@ -4856,7 +4868,7 @@
       <c r="F65" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G65" s="30" t="s">
+      <c r="G65" s="32" t="s">
         <v>137</v>
       </c>
       <c r="H65" s="15" t="s">
@@ -4864,7 +4876,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="6" t="s">
         <v>220</v>
       </c>
@@ -4880,13 +4892,13 @@
       <c r="F66" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G66" s="30"/>
+      <c r="G66" s="32"/>
       <c r="H66" s="15" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="42"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="6" t="s">
         <v>221</v>
       </c>
@@ -4902,13 +4914,13 @@
       <c r="F67" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G67" s="30"/>
+      <c r="G67" s="32"/>
       <c r="H67" s="15" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="42">
+      <c r="A68" s="26">
         <v>23</v>
       </c>
       <c r="B68" s="6" t="s">
@@ -4926,7 +4938,7 @@
       <c r="F68" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G68" s="30" t="s">
+      <c r="G68" s="32" t="s">
         <v>143</v>
       </c>
       <c r="H68" s="15" t="s">
@@ -4934,7 +4946,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="42"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="6" t="s">
         <v>223</v>
       </c>
@@ -4950,13 +4962,13 @@
       <c r="F69" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G69" s="30"/>
+      <c r="G69" s="32"/>
       <c r="H69" s="15" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="42"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="6" t="s">
         <v>224</v>
       </c>
@@ -4972,7 +4984,7 @@
       <c r="F70" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G70" s="30" t="s">
+      <c r="G70" s="32" t="s">
         <v>150</v>
       </c>
       <c r="H70" s="15" t="s">
@@ -4980,7 +4992,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="42">
+      <c r="A71" s="26">
         <v>24</v>
       </c>
       <c r="B71" s="6" t="s">
@@ -4998,13 +5010,13 @@
       <c r="F71" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G71" s="30"/>
+      <c r="G71" s="32"/>
       <c r="H71" s="15" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="42"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="6" t="s">
         <v>226</v>
       </c>
@@ -5028,7 +5040,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A73" s="42"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="9">
         <v>44927</v>
       </c>
@@ -5044,7 +5056,7 @@
       <c r="F73" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G73" s="43" t="s">
+      <c r="G73" s="33" t="s">
         <v>156</v>
       </c>
       <c r="H73" s="15" t="s">
@@ -5052,7 +5064,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A74" s="42">
+      <c r="A74" s="26">
         <v>25</v>
       </c>
       <c r="B74" s="9">
@@ -5070,13 +5082,13 @@
       <c r="F74" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G74" s="43"/>
+      <c r="G74" s="33"/>
       <c r="H74" s="15" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="42"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="9">
         <v>45108</v>
       </c>
@@ -5092,7 +5104,7 @@
       <c r="F75" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G75" s="30" t="s">
+      <c r="G75" s="32" t="s">
         <v>169</v>
       </c>
       <c r="H75" s="15" t="s">
@@ -5100,7 +5112,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="42"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="9">
         <v>45139</v>
       </c>
@@ -5116,13 +5128,13 @@
       <c r="F76" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G76" s="28"/>
+      <c r="G76" s="34"/>
       <c r="H76" s="15" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="42">
+      <c r="A77" s="26">
         <v>26</v>
       </c>
       <c r="B77" s="6" t="s">
@@ -5140,13 +5152,13 @@
       <c r="F77" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G77" s="28"/>
+      <c r="G77" s="34"/>
       <c r="H77" s="15" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="42"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="6" t="s">
         <v>228</v>
       </c>
@@ -5162,15 +5174,15 @@
       <c r="F78" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G78" s="40" t="s">
+      <c r="G78" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="H78" s="40" t="s">
+      <c r="H78" s="30" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="42"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="6" t="s">
         <v>229</v>
       </c>
@@ -5186,11 +5198,11 @@
       <c r="F79" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G79" s="40"/>
-      <c r="H79" s="40"/>
+      <c r="G79" s="30"/>
+      <c r="H79" s="30"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="42">
+      <c r="A80" s="26">
         <v>27</v>
       </c>
       <c r="B80" s="6" t="s">
@@ -5208,13 +5220,13 @@
       <c r="F80" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G80" s="40"/>
-      <c r="H80" s="37" t="s">
+      <c r="G80" s="30"/>
+      <c r="H80" s="27" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="42"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="6" t="s">
         <v>292</v>
       </c>
@@ -5230,11 +5242,11 @@
       <c r="F81" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G81" s="40"/>
-      <c r="H81" s="38"/>
+      <c r="G81" s="30"/>
+      <c r="H81" s="28"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="42"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="6" t="s">
         <v>293</v>
       </c>
@@ -5250,31 +5262,34 @@
       <c r="F82" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G82" s="40"/>
-      <c r="H82" s="39"/>
+      <c r="G82" s="30"/>
+      <c r="H82" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="E20:E23" xr:uid="{AE790FB6-A56C-104E-ADFC-0FABBBB49FA5}"/>
   <mergeCells count="57">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G35:G40"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="G28:G33"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="G49:G52"/>
+    <mergeCell ref="G53:G56"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G45:G47"/>
     <mergeCell ref="H80:H82"/>
     <mergeCell ref="H78:H79"/>
     <mergeCell ref="A2:A4"/>
@@ -5291,28 +5306,25 @@
     <mergeCell ref="G59:G60"/>
     <mergeCell ref="G61:G62"/>
     <mergeCell ref="A56:A58"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="G49:G52"/>
-    <mergeCell ref="G53:G56"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="G45:G47"/>
-    <mergeCell ref="G35:G40"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="G28:G33"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A74:A76"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>